<commit_message>
changes to test and data
</commit_message>
<xml_diff>
--- a/src/main/java/com/fin/qa/testdata/FinTestdata.xlsx
+++ b/src/main/java/com/fin/qa/testdata/FinTestdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="details" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>firstname</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>super@grr.la</t>
+  </si>
+  <si>
+    <t>finleaptesto@grr.la</t>
   </si>
 </sst>
 </file>
@@ -383,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -414,7 +417,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -466,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>